<commit_message>
Push de la journée
Ajout du MCD, du MLD, mise à jour de la documentation et du journal de bord
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravailMPI.xlsx
+++ b/Documentation/journalDeTravailMPI.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,78 @@
   </si>
   <si>
     <t>Écriture du premier mail avec toutes les informations pour lancer le projet. (différents liens, planification initial, etc…)</t>
+  </si>
+  <si>
+    <t>Analyse concurentielle</t>
+  </si>
+  <si>
+    <t>Analyse concurentielle pour le produit faite et ajoutée à la documentation</t>
+  </si>
+  <si>
+    <t>Étude de faisabilité</t>
+  </si>
+  <si>
+    <t>Ajout de l'étude de faisabilité effectuée dans la documentation</t>
+  </si>
+  <si>
+    <t>Choix du nom de domaine et du site</t>
+  </si>
+  <si>
+    <t>Intégration de la planification détaillé</t>
+  </si>
+  <si>
+    <t>Intégration de la planification détaillée dans la documentation</t>
+  </si>
+  <si>
+    <t>Analyse de l'environnement</t>
+  </si>
+  <si>
+    <t>Ajout du résultat de l'analyse de l'environnement dans la documentation</t>
+  </si>
+  <si>
+    <t>Création MCD</t>
+  </si>
+  <si>
+    <t>Analyse et création du MCD, ajout de ce dernier dans la documentation</t>
+  </si>
+  <si>
+    <t>Création MLD</t>
+  </si>
+  <si>
+    <t>Analyse et création du MLD, sur les bases du MCD, ajout de ce dernier dans la documentation</t>
+  </si>
+  <si>
+    <t>Création des cas d'utilisation</t>
+  </si>
+  <si>
+    <t>Commencement de l'ajout des cas d'utilisation à la documentation</t>
+  </si>
+  <si>
+    <t>Création de l'arborescence du site</t>
+  </si>
+  <si>
+    <t>Définition de la charte graphique</t>
+  </si>
+  <si>
+    <t>Analyse et réalisation de la charte graphique du site, ajout dans la documentation</t>
+  </si>
+  <si>
+    <t>Analyse et réalisation de l'arborescence du site et ajout de ces informations dans la documentation</t>
+  </si>
+  <si>
+    <t>Fin des cas d'utilisation</t>
+  </si>
+  <si>
+    <t>Ajout de différents cas d'utilisation pour clôturer ce point</t>
+  </si>
+  <si>
+    <t>Avancement des maquettes graphiques</t>
+  </si>
+  <si>
+    <t>Ajout de proposition pour le nom de domaine et du site web dans la documentation et vérification pour savoir si les noms de domaines étaient libres</t>
+  </si>
+  <si>
+    <t>Maquettes graphiques</t>
   </si>
 </sst>
 </file>
@@ -310,38 +382,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -362,22 +407,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -395,7 +467,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0\ &quot;minutes&quot;"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
@@ -413,7 +485,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
@@ -430,7 +502,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -508,13 +580,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F80" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="C2:F80"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Tâche" dataDxfId="3"/>
-    <tableColumn id="3" name="Date" dataDxfId="2"/>
-    <tableColumn id="4" name="Temps" dataDxfId="1"/>
-    <tableColumn id="5" name="Description supplémentaire" dataDxfId="0"/>
+    <tableColumn id="1" name="Tâche" dataDxfId="4"/>
+    <tableColumn id="3" name="Date" dataDxfId="3"/>
+    <tableColumn id="4" name="Temps" dataDxfId="2"/>
+    <tableColumn id="5" name="Description supplémentaire" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -788,8 +860,8 @@
   </sheetPr>
   <dimension ref="B1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,562 +893,658 @@
       </c>
     </row>
     <row r="3" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="15">
         <v>44319</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="16">
         <v>45</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="18">
         <v>44319</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="19">
         <v>30</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="18">
         <v>44319</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="20">
         <v>30</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="21">
         <v>44319</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="20">
         <v>20</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="21">
         <v>44319</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="20">
         <v>70</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="21"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="21">
         <v>44319</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="20">
         <v>20</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="21">
         <v>44319</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="20">
         <v>60</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="21">
         <v>44319</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="20">
         <v>30</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="21">
         <v>44319</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="20">
         <v>60</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="21">
         <v>44319</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="20">
         <v>20</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="19"/>
+      <c r="C13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E13" s="20">
+        <v>15</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="19"/>
+      <c r="C14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E14" s="20">
+        <v>10</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E15" s="20">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E16" s="20">
+        <v>10</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="19"/>
+      <c r="C17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E17" s="20">
+        <v>20</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="19"/>
+      <c r="C18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E18" s="20">
+        <v>60</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="19"/>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="19"/>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="19"/>
+      <c r="C19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E19" s="20">
+        <v>40</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E20" s="20">
+        <v>60</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E21" s="20">
+        <v>10</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E22" s="20">
+        <v>15</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="19"/>
+      <c r="C23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E23" s="20">
+        <v>30</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="19"/>
+      <c r="C24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="21">
+        <v>44320</v>
+      </c>
+      <c r="E24" s="20">
+        <v>60</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="19"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="19"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="19"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="19"/>
-      <c r="H28" s="21"/>
-      <c r="O28" s="21"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="10"/>
+      <c r="H28" s="11"/>
+      <c r="O28" s="11"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="19"/>
-      <c r="O29" s="21"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="10"/>
+      <c r="O29" s="11"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="19"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="19"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="19"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="19"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="19"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="19"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="19"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="10"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="19"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="19"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="19"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="10"/>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="19"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="10"/>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="19"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="19"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="7"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="19"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="7"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="19"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="10"/>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="7"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="19"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="19"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="10"/>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="7"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="19"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="10"/>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="7"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="22"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="12"/>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="22"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="12"/>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" s="7"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="22"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="12"/>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="22"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="12"/>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="7"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="22"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="12"/>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="7"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="19"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="10"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="7"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="19"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="10"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="7"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="19"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="10"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="7"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="19"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="10"/>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="7"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="19"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="10"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="7"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="19"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="10"/>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="7"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="19"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="10"/>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="7"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="19"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="10"/>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="7"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="19"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="10"/>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="7"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="19"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="10"/>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="7"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="19"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="10"/>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="7"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="19"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="10"/>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="19"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="10"/>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C66" s="7"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="19"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="10"/>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C67" s="7"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="19"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="10"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="7"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="19"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="10"/>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="7"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="19"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="10"/>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C70" s="7"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="19"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="10"/>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C71" s="7"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="19"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="10"/>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C72" s="7"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="19"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="10"/>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C73" s="7"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="19"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="10"/>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C74" s="7"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="19"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="10"/>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C75" s="7"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="19"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="10"/>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C76" s="23"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="19"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="10"/>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C77" s="7"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="19"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="10"/>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C78" s="7"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="19"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="10"/>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="7"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="19"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="10"/>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C81" s="13"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="16"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout d'éléments nécessaire à l'analyse et la conception du site
Ajout de toutes les maquettes graphiques, mise à jour du rapport, avec ajout des stratégies de test. Ajout d'un historique du projet et d'une description pour la planification initiale et détaillée du projet.
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravailMPI.xlsx
+++ b/Documentation/journalDeTravailMPI.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,33 @@
   </si>
   <si>
     <t>Maquettes graphiques</t>
+  </si>
+  <si>
+    <t>Ajout de description dans le rapport pour la planification initale et détaillée</t>
+  </si>
+  <si>
+    <t>Méthodologie de travail</t>
+  </si>
+  <si>
+    <t>Ajout de la description de la méthodologie de travail utilisée dans le rapport</t>
+  </si>
+  <si>
+    <t>Ajout de nouvelles maquettes graphiques et finalisation de ces dernières, export en PDF et PNG</t>
+  </si>
+  <si>
+    <t>Ajout des maquettes grpahiques des fonctionnalités les plus "importantes" dans le rapport</t>
+  </si>
+  <si>
+    <t>Discussion avec chef de projet</t>
+  </si>
+  <si>
+    <t>Discussion avec Monsieur Benzonana, par rapport au cahier des charges, modification et signature du cahier des charges modifiés</t>
+  </si>
+  <si>
+    <t>Ajout d'un historique dans le rapport de projet par rapport à la modification du cahier des charges</t>
+  </si>
+  <si>
+    <t>Ajout des stratégies de test à la documentation</t>
   </si>
 </sst>
 </file>
@@ -448,9 +475,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -531,6 +555,9 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -580,13 +607,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <autoFilter ref="C2:F80"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Tâche" dataDxfId="4"/>
-    <tableColumn id="3" name="Date" dataDxfId="3"/>
-    <tableColumn id="4" name="Temps" dataDxfId="2"/>
-    <tableColumn id="5" name="Description supplémentaire" dataDxfId="1"/>
+    <tableColumn id="1" name="Tâche" dataDxfId="3"/>
+    <tableColumn id="3" name="Date" dataDxfId="2"/>
+    <tableColumn id="4" name="Temps" dataDxfId="1"/>
+    <tableColumn id="5" name="Description supplémentaire" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -860,8 +887,8 @@
   </sheetPr>
   <dimension ref="B1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,49 +1229,105 @@
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="13"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="10"/>
+      <c r="C25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="21">
+        <v>44322</v>
+      </c>
+      <c r="E25" s="20">
+        <v>15</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="13"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="13"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="13"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="10"/>
+      <c r="C26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="21">
+        <v>44322</v>
+      </c>
+      <c r="E26" s="20">
+        <v>5</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="21">
+        <v>44322</v>
+      </c>
+      <c r="E27" s="20">
+        <v>120</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="21">
+        <v>44322</v>
+      </c>
+      <c r="E28" s="20">
+        <v>20</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="H28" s="11"/>
       <c r="O28" s="11"/>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="13"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="10"/>
+    <row r="29" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="21">
+        <v>44322</v>
+      </c>
+      <c r="E29" s="20">
+        <v>15</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="O29" s="11"/>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="13"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="10"/>
+    <row r="30" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="21">
+        <v>44322</v>
+      </c>
+      <c r="E30" s="20">
+        <v>5</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="13"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="10"/>
+      <c r="C31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="21">
+        <v>44322</v>
+      </c>
+      <c r="E31" s="20">
+        <v>55</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" s="13"/>

</xml_diff>

<commit_message>
Création script BD + commencement fonction login
Création du script pour la création de la DB, ajout de l'implémentation d'un template. Création de la page de login. Commencement des fonctions de nécessaires au login des users
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravailMPI.xlsx
+++ b/Documentation/journalDeTravailMPI.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Explication du déroulement du TPI par Monsieur Montemayor et explication des attentes.</t>
   </si>
   <si>
-    <t>Mise en place de l'hébergement web, ainsi que de l'hébergement pour la base de données</t>
-  </si>
-  <si>
     <t>Création de la plannification initial</t>
   </si>
   <si>
@@ -204,6 +201,66 @@
   </si>
   <si>
     <t>Ajout des stratégies de test à la documentation</t>
+  </si>
+  <si>
+    <t>Création de la base MVC</t>
+  </si>
+  <si>
+    <t>Création de toute la base MVC du projet</t>
+  </si>
+  <si>
+    <t>Préparation des fichiers</t>
+  </si>
+  <si>
+    <t>Préparation de tous les fichiers nécessaires à la création du projet. Ajout des noms de fonctions de base, etc…</t>
+  </si>
+  <si>
+    <t>Sélection d'un template</t>
+  </si>
+  <si>
+    <t>Sélection d'un template adéquat pour pouvoir par la suite le modifier et l'utiliser pour la réalisation de mon projet</t>
+  </si>
+  <si>
+    <t>Création d'un serveur web de test afin de pouvoir tester l'avancée du projet sans pour autant impacter le serveur web fonctionnel</t>
+  </si>
+  <si>
+    <t>Mise en place de l'hébergement web pour le serveur web fonctionnel, ainsi que de l'hébergement pour la base de données</t>
+  </si>
+  <si>
+    <t>Modification template</t>
+  </si>
+  <si>
+    <t>Modification du template afin d'avoir un premier point de vue, le plus ressemblant possible aux maquettes créées</t>
+  </si>
+  <si>
+    <t>Modification fonction</t>
+  </si>
+  <si>
+    <t>Modification des premières fonctions créées précédemment, afin de pouvoir dans un premier temps accéder à la page de login et d'accueil</t>
+  </si>
+  <si>
+    <t>Ajout de la page de login</t>
+  </si>
+  <si>
+    <t>Création du code nécessaire à la page de login</t>
+  </si>
+  <si>
+    <t>Intégration du template</t>
+  </si>
+  <si>
+    <t>Intégration du template dans le code afin d'avoir un premier point de vue, fonctionnel</t>
+  </si>
+  <si>
+    <t>Création de la base de données</t>
+  </si>
+  <si>
+    <t>Création du script nécessaire à la création de la structure de la base de données du projet</t>
+  </si>
+  <si>
+    <t>Création fonction de login</t>
+  </si>
+  <si>
+    <t>Création des diverses fonctions nécessaire à la fonction de login. Pour l'instant la fonctionnalité n'est pas encore fonctionnel.</t>
   </si>
 </sst>
 </file>
@@ -409,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -426,9 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -442,15 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -467,6 +512,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -607,8 +667,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
-  <autoFilter ref="C2:F80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F82" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="C2:F82"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tâche" dataDxfId="3"/>
     <tableColumn id="3" name="Date" dataDxfId="2"/>
@@ -885,10 +945,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O81"/>
+  <dimension ref="B1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,715 +979,809 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="14" t="s">
+    <row r="3" spans="3:9" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="20"/>
+      <c r="D3" s="19">
+        <v>44319</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D4" s="14">
         <v>44319</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E4" s="15">
         <v>45</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="17" t="s">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D5" s="14">
         <v>44319</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E5" s="15">
         <v>30</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="13" t="s">
+    <row r="6" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D6" s="14">
         <v>44319</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E6" s="16">
         <v>30</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="13" t="s">
+    <row r="7" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D7" s="17">
         <v>44319</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E7" s="16">
         <v>20</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F7" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
+      <c r="D8" s="17">
+        <v>44319</v>
+      </c>
+      <c r="E8" s="16">
+        <v>70</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="21">
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="17">
         <v>44319</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E9" s="16">
+        <v>20</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="17">
+        <v>44319</v>
+      </c>
+      <c r="E10" s="16">
+        <v>60</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="17">
+        <v>44319</v>
+      </c>
+      <c r="E11" s="16">
+        <v>30</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="17">
+        <v>44319</v>
+      </c>
+      <c r="E12" s="16">
+        <v>60</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="17">
+        <v>44319</v>
+      </c>
+      <c r="E13" s="16">
+        <v>20</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="12"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E15" s="16">
+        <v>15</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E16" s="16">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E17" s="16">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E18" s="16">
+        <v>10</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E19" s="16">
+        <v>20</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E20" s="16">
+        <v>60</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E21" s="16">
+        <v>40</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E22" s="16">
+        <v>60</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E23" s="16">
+        <v>10</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E24" s="16">
+        <v>15</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E25" s="16">
+        <v>30</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="17">
+        <v>44320</v>
+      </c>
+      <c r="E26" s="16">
+        <v>60</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E27" s="16">
+        <v>15</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E28" s="16">
+        <v>5</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E29" s="16">
+        <v>120</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E30" s="16">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="O30" s="10"/>
+    </row>
+    <row r="31" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E31" s="16">
+        <v>15</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="O31" s="10"/>
+    </row>
+    <row r="32" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E32" s="16">
+        <v>5</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E33" s="16">
+        <v>55</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E34" s="16">
+        <v>30</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C35" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E35" s="16">
+        <v>120</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="17">
+        <v>44322</v>
+      </c>
+      <c r="E36" s="16">
+        <v>20</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="17">
+        <v>44323</v>
+      </c>
+      <c r="E37" s="16">
+        <v>10</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="17">
+        <v>44323</v>
+      </c>
+      <c r="E38" s="16">
+        <v>45</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="17">
+        <v>44323</v>
+      </c>
+      <c r="E39" s="16">
+        <v>15</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="17">
+        <v>44323</v>
+      </c>
+      <c r="E40" s="16">
+        <v>10</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C41" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="21">
-        <v>44319</v>
-      </c>
-      <c r="E8" s="20">
-        <v>20</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="21">
-        <v>44319</v>
-      </c>
-      <c r="E9" s="20">
-        <v>60</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="21">
-        <v>44319</v>
-      </c>
-      <c r="E10" s="20">
-        <v>30</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="21">
-        <v>44319</v>
-      </c>
-      <c r="E11" s="20">
-        <v>60</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="21">
-        <v>44319</v>
-      </c>
-      <c r="E12" s="20">
-        <v>20</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E13" s="20">
-        <v>15</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E14" s="20">
+      <c r="D41" s="17">
+        <v>44323</v>
+      </c>
+      <c r="E41" s="16">
         <v>10</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E15" s="20">
-        <v>10</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E16" s="20">
-        <v>10</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E17" s="20">
-        <v>20</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E18" s="20">
-        <v>60</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E19" s="20">
-        <v>40</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E20" s="20">
-        <v>60</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E21" s="20">
-        <v>10</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E22" s="20">
-        <v>15</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E23" s="20">
-        <v>30</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="21">
-        <v>44320</v>
-      </c>
-      <c r="E24" s="20">
-        <v>60</v>
-      </c>
-      <c r="F24" s="10" t="s">
+      <c r="F41" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="17">
+        <v>44323</v>
+      </c>
+      <c r="E42" s="16">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="21">
-        <v>44322</v>
-      </c>
-      <c r="E25" s="20">
-        <v>15</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="21">
-        <v>44322</v>
-      </c>
-      <c r="E26" s="20">
-        <v>5</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="21">
-        <v>44322</v>
-      </c>
-      <c r="E27" s="20">
-        <v>120</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="21">
-        <v>44322</v>
-      </c>
-      <c r="E28" s="20">
-        <v>20</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="11"/>
-      <c r="O28" s="11"/>
-    </row>
-    <row r="29" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C29" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="21">
-        <v>44322</v>
-      </c>
-      <c r="E29" s="20">
-        <v>15</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O29" s="11"/>
-    </row>
-    <row r="30" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C30" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="21">
-        <v>44322</v>
-      </c>
-      <c r="E30" s="20">
-        <v>5</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="21">
-        <v>44322</v>
-      </c>
-      <c r="E31" s="20">
-        <v>55</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="13"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="13"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="13"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="10"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="13"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="13"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="13"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="13"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="13"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="10"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="13"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="10"/>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="13"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="13"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="10"/>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="13"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="10"/>
+      <c r="F42" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C43" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="17">
+        <v>44323</v>
+      </c>
+      <c r="E43" s="16">
+        <v>45</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="13"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="10"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="13"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="10"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="13"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="10"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="13"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="10"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="13"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="13"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" s="13"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="11"/>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="13"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="13"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="13"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="10"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="11"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="13"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="10"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="11"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="13"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="10"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="13"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="10"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="13"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="10"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="13"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="10"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="13"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="10"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="13"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="10"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="13"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="10"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="9"/>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="13"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="10"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="9"/>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="13"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="10"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="9"/>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="13"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="10"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="9"/>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C65" s="13"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="10"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="9"/>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C66" s="13"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="10"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="9"/>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C67" s="13"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="10"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="9"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="13"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="10"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="9"/>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="13"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="10"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="9"/>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C70" s="13"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="10"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C71" s="13"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="10"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="9"/>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C72" s="13"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="10"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="9"/>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C73" s="13"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="10"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="9"/>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C74" s="13"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="10"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="9"/>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C75" s="13"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="10"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="9"/>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C76" s="13"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="10"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="9"/>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C77" s="13"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="10"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="9"/>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C78" s="13"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="10"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="9"/>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="13"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="10"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="9"/>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="9"/>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C81" s="4"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="7"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="9"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="18"/>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C83" s="4"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mise à jour de la documentation et du journal de travail
Mise à jour de ces documents et préparation du rendu de semaine.
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravailMPI.xlsx
+++ b/Documentation/journalDeTravailMPI.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="138">
   <si>
     <t>Date</t>
   </si>
@@ -372,6 +372,81 @@
   </si>
   <si>
     <t>Construction de la page d'accueil, beaucoup de temps passer à faire en sorte d'avoir un environnement le plus responsive possible et pour faire en sorte d'avoir quelque chose qui ressemble le plus possible aux maquettes</t>
+  </si>
+  <si>
+    <t>Modification page d'accueil</t>
+  </si>
+  <si>
+    <t>Dernière modification visuel pour la page d'accueil</t>
+  </si>
+  <si>
+    <t>Modification du template de base afin d'avoir un visuel correspondant aux maquettes</t>
+  </si>
+  <si>
+    <t>ajout de notifications</t>
+  </si>
+  <si>
+    <t>J'ai passé pas mal de temps à me réhabituer avec les nouvelles fonctionnalités des modals d'informations de bootstrap V5. Après cela j'ai pu me concentrer sur la réalisation des notifications de connexion utilisateur</t>
+  </si>
+  <si>
+    <t>Modifications cases consommables</t>
+  </si>
+  <si>
+    <t>Ajout de modal</t>
+  </si>
+  <si>
+    <t>Création des différentes modals pour les fonctions de tris</t>
+  </si>
+  <si>
+    <t>Mise à jour documentation</t>
+  </si>
+  <si>
+    <t>Définition et ajout d'un niveau d'incidence pour les stratégies de test</t>
+  </si>
+  <si>
+    <t>Modifications des cases pour les consommables, afin d'obtenir un aspect visuel plus ressemblants aux maquettes et amélioration de la navigation web (plus résponsive). Cela m'a pris du temps parce que j'ai butté sur des petits détails</t>
+  </si>
+  <si>
+    <t>Sprint rétrospective du second sprint avec le chef de projet. Nous avons parlé essentiellements de l'avancée du projet et du code en général.</t>
+  </si>
+  <si>
+    <t>Sprint rétrospective</t>
+  </si>
+  <si>
+    <t>Ajout sprint review</t>
+  </si>
+  <si>
+    <t>Création de la sprint review numéro 2, disponible sur le wiki du dépôt github du projet</t>
+  </si>
+  <si>
+    <t>Mise à jour Trello</t>
+  </si>
+  <si>
+    <t>Mise à jour du Trello suite à la discussion avec le chef de projet</t>
+  </si>
+  <si>
+    <t>Ajout de consommables</t>
+  </si>
+  <si>
+    <t>Ajout de consommables à la base de données, avec toutes les relations nécessaires et je me suis rendu compte de plusieurs erreurs dans la structure de la base de données modifications effectuées dans l'historique</t>
+  </si>
+  <si>
+    <t>Création vue sur la BD</t>
+  </si>
+  <si>
+    <t>Mise en place d'une vue afin de faciliter la sélection des différentes données pour l'affichage. Cela m'a pris passablement de temps et mon collègues Jérôme Jaquemet m'a aidé dans la réalisation de certaines commandes</t>
+  </si>
+  <si>
+    <t>Création fonction récupération des données</t>
+  </si>
+  <si>
+    <t>Création des fonctions de récupération des données nécessaires sur la page d'accueil, que ce soit pour les consommables ou pour les différentes options de tri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en forme des données </t>
+  </si>
+  <si>
+    <t>Mise en forme des données récupérées par les fonctions crééer précédemment</t>
   </si>
 </sst>
 </file>
@@ -725,8 +800,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
-  <autoFilter ref="C2:F80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F88" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="C2:F88"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tâche" dataDxfId="3"/>
     <tableColumn id="3" name="Date" dataDxfId="2"/>
@@ -1003,10 +1078,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O81"/>
+  <dimension ref="B1:O89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,82 +1929,186 @@
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="12"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="9"/>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="12"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="12"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="9"/>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="12"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="9"/>
+      <c r="C61" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" s="17">
+        <v>44333</v>
+      </c>
+      <c r="E61" s="16">
+        <v>60</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C62" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="17">
+        <v>44333</v>
+      </c>
+      <c r="E62" s="16">
+        <v>45</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C63" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D63" s="17">
+        <v>44333</v>
+      </c>
+      <c r="E63" s="16">
+        <v>90</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C64" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="17">
+        <v>44333</v>
+      </c>
+      <c r="E64" s="16">
+        <v>110</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C65" s="12"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="9"/>
+      <c r="C65" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" s="17">
+        <v>44333</v>
+      </c>
+      <c r="E65" s="16">
+        <v>45</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C66" s="12"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="9"/>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C67" s="12"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="9"/>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="12"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="9"/>
+      <c r="C66" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" s="17">
+        <v>44333</v>
+      </c>
+      <c r="E66" s="16">
+        <v>20</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C67" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="17">
+        <v>44334</v>
+      </c>
+      <c r="E67" s="16">
+        <v>40</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C68" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D68" s="17">
+        <v>44334</v>
+      </c>
+      <c r="E68" s="16">
+        <v>30</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="12"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="9"/>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C70" s="12"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="9"/>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C71" s="12"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="9"/>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C72" s="12"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="9"/>
+      <c r="C69" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" s="17">
+        <v>44334</v>
+      </c>
+      <c r="E69" s="16">
+        <v>5</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C70" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D70" s="17">
+        <v>44334</v>
+      </c>
+      <c r="E70" s="16">
+        <v>85</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C71" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="17">
+        <v>44334</v>
+      </c>
+      <c r="E71" s="16">
+        <v>90</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C72" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D72" s="17">
+        <v>44334</v>
+      </c>
+      <c r="E72" s="16">
+        <v>50</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C73" s="12"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="9"/>
+      <c r="C73" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D73" s="17">
+        <v>44334</v>
+      </c>
+      <c r="E73" s="16">
+        <v>60</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" s="12"/>
@@ -1968,16 +2147,64 @@
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="18"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="9"/>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C81" s="4"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="7"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="9"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="12"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="9"/>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C83" s="12"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="9"/>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C84" s="12"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="9"/>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C85" s="12"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="9"/>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C86" s="12"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="9"/>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C87" s="12"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="9"/>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="18"/>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C89" s="4"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Préparation des fonctions nécessaires pour la page admin
Création des différentes fonctions et mise à jour de la documentation pour le pointage de semaine
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravailMPI.xlsx
+++ b/Documentation/journalDeTravailMPI.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="176">
   <si>
     <t>Date</t>
   </si>
@@ -407,12 +407,6 @@
     <t>Modifications des cases pour les consommables, afin d'obtenir un aspect visuel plus ressemblants aux maquettes et amélioration de la navigation web (plus résponsive). Cela m'a pris du temps parce que j'ai butté sur des petits détails</t>
   </si>
   <si>
-    <t>Sprint rétrospective du second sprint avec le chef de projet. Nous avons parlé essentiellements de l'avancée du projet et du code en général.</t>
-  </si>
-  <si>
-    <t>Sprint rétrospective</t>
-  </si>
-  <si>
     <t>Ajout sprint review</t>
   </si>
   <si>
@@ -482,9 +476,6 @@
     <t>Recherche et apprentissage</t>
   </si>
   <si>
-    <t>Recherche et apprentissage sur l'envoie dynamique de commande PHP via JS et l'utilisation de la méthode XMLHtppRequest, lien qui m'a été particulièrement utile lors de mes recherches : https://developer.mozilla.org/fr/docs/Learn/Forms/Sending_forms_through_JavaScript</t>
-  </si>
-  <si>
     <t>Fonction sauvegarde des stock</t>
   </si>
   <si>
@@ -531,6 +522,65 @@
   </si>
   <si>
     <t>Mise à jour des nouveaux éléments, sauf les maquettes qui ne sont pas encore ajoutées à la doc</t>
+  </si>
+  <si>
+    <t>Correction fonction dynamique</t>
+  </si>
+  <si>
+    <t>Correction de la fonction dynamique qui posait problème sur le serveur de production. Ajout d'un élément de la fonctionnalité oublié qui permet de sauvegarder les différentes actions dans la base de données. J'ai rencontré quelques problèmes à ce sujet notamment du au fait que je n'arrivai pas à récupérer la session lors du call de la fonction php. Le problème a été contourné et résolu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Recherche et apprentissage sur l'envoie dynamique de commande PHP via JS et l'utilisation de la méthode XMLHtppRequest, lien qui m'a été particulièrement utile lors de mes recherches : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://developer.mozilla.org/fr/docs/Learn/Forms/Sending_forms_throug</t>
+    </r>
+  </si>
+  <si>
+    <t>Création de la vue admin</t>
+  </si>
+  <si>
+    <t>Création de tous les éléments nécessaires à la page de gestionnaire administrateur. Création du visuel respectant la maquette créé au préalable. Mise en place de fonction permettant la récupération des données. Et affichage de ces données.</t>
+  </si>
+  <si>
+    <t>Préparation des fonctions nécessaire page admin</t>
+  </si>
+  <si>
+    <t>Préparation des fonctions qui seront nécessaires pour le bon fonctionnement des différentes fonctionnalités disponibles sur la page de gestionnaire administrateur.</t>
+  </si>
+  <si>
+    <t>Création sprint rétrospective3</t>
+  </si>
+  <si>
+    <t>Rendez-vous M. Benzonana</t>
+  </si>
+  <si>
+    <t>Sprint review</t>
+  </si>
+  <si>
+    <t>Sprint review du second sprint avec le chef de projet. Nous avons parlé essentiellements de l'avancée du projet et du code en général.</t>
+  </si>
+  <si>
+    <t>Sprint review avec le chef de projet. Lors de cet entretien nous avons essentiellement parler de l'avancée en général du projet.</t>
+  </si>
+  <si>
+    <t>Création de la sprint rétrospective numéro 3, disponible sur le wiki du dépôt github pour plus d'information</t>
   </si>
 </sst>
 </file>
@@ -540,7 +590,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0\ &quot;minutes&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +602,14 @@
       <b/>
       <sz val="22"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -692,10 +750,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -743,14 +802,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -834,6 +894,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thick">
           <color auto="1"/>
@@ -881,13 +944,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F95" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="C2:F95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C2:F94" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="C2:F94"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Tâche" dataDxfId="4"/>
-    <tableColumn id="3" name="Date" dataDxfId="3"/>
-    <tableColumn id="4" name="Temps" dataDxfId="2"/>
-    <tableColumn id="5" name="Description supplémentaire" dataDxfId="1"/>
+    <tableColumn id="1" name="Tâche" dataDxfId="3"/>
+    <tableColumn id="3" name="Date" dataDxfId="2"/>
+    <tableColumn id="4" name="Temps" dataDxfId="1"/>
+    <tableColumn id="5" name="Description supplémentaire" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1159,10 +1222,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O96"/>
+  <dimension ref="B1:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2158,7 @@
     </row>
     <row r="67" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C67" s="11" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="D67" s="16">
         <v>44334</v>
@@ -2104,12 +2167,12 @@
         <v>40</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C68" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D68" s="16">
         <v>44334</v>
@@ -2118,12 +2181,12 @@
         <v>30</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D69" s="16">
         <v>44334</v>
@@ -2132,12 +2195,12 @@
         <v>5</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C70" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D70" s="16">
         <v>44334</v>
@@ -2146,12 +2209,12 @@
         <v>85</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C71" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D71" s="16">
         <v>44334</v>
@@ -2160,12 +2223,12 @@
         <v>90</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C72" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D72" s="16">
         <v>44334</v>
@@ -2174,12 +2237,12 @@
         <v>50</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D73" s="16">
         <v>44334</v>
@@ -2188,12 +2251,12 @@
         <v>60</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C74" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D74" s="16">
         <v>44336</v>
@@ -2202,12 +2265,12 @@
         <v>80</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C75" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D75" s="16">
         <v>44336</v>
@@ -2216,12 +2279,12 @@
         <v>20</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C76" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D76" s="16">
         <v>44336</v>
@@ -2230,12 +2293,12 @@
         <v>80</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C77" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D77" s="16">
         <v>44336</v>
@@ -2244,12 +2307,12 @@
         <v>10</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C78" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D78" s="16">
         <v>44336</v>
@@ -2258,12 +2321,12 @@
         <v>10</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="79" spans="3:6" ht="75" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6" ht="60" x14ac:dyDescent="0.25">
       <c r="C79" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D79" s="16">
         <v>44336</v>
@@ -2271,13 +2334,13 @@
       <c r="E79" s="15">
         <v>60</v>
       </c>
-      <c r="F79" s="9" t="s">
-        <v>149</v>
+      <c r="F79" s="19" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C80" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D80" s="16">
         <v>44336</v>
@@ -2286,12 +2349,12 @@
         <v>60</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C81" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D81" s="16">
         <v>44336</v>
@@ -2300,12 +2363,12 @@
         <v>30</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C82" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D82" s="16">
         <v>44336</v>
@@ -2314,12 +2377,12 @@
         <v>60</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="83" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C83" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D83" s="16">
         <v>44336</v>
@@ -2328,12 +2391,12 @@
         <v>20</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C84" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D84" s="16">
         <v>44337</v>
@@ -2342,12 +2405,12 @@
         <v>90</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C85" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D85" s="16">
         <v>44337</v>
@@ -2356,12 +2419,12 @@
         <v>15</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C86" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D86" s="16">
         <v>44337</v>
@@ -2370,7 +2433,7 @@
         <v>45</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.25">
@@ -2384,7 +2447,7 @@
         <v>35</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="88" spans="3:6" ht="30" x14ac:dyDescent="0.25">
@@ -2398,62 +2461,99 @@
         <v>10</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C89" s="11"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="15"/>
-      <c r="F89" s="9"/>
-    </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C90" s="11"/>
-      <c r="D90" s="16"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="9"/>
-    </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C91" s="11"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="15"/>
-      <c r="F91" s="9"/>
-    </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C92" s="11"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="15"/>
-      <c r="F92" s="9"/>
-    </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C93" s="11"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="15"/>
-      <c r="F93" s="9"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C89" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D89" s="16">
+        <v>44338</v>
+      </c>
+      <c r="E89" s="15">
+        <v>35</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="C90" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D90" s="16">
+        <v>44341</v>
+      </c>
+      <c r="E90" s="15">
+        <v>100</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C91" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" s="16">
+        <v>44341</v>
+      </c>
+      <c r="E91" s="15">
+        <v>90</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C92" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D92" s="16">
+        <v>44341</v>
+      </c>
+      <c r="E92" s="15">
+        <v>50</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C93" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D93" s="16">
+        <v>44341</v>
+      </c>
+      <c r="E93" s="15">
+        <v>20</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="94" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="11"/>
-      <c r="D94" s="16"/>
-      <c r="E94" s="15"/>
-      <c r="F94" s="9"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="17"/>
     </row>
     <row r="95" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="17"/>
-    </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C96" s="4"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="7"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F79" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="152" scale="69" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="152" scale="69" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>